<commit_message>
Updated accueil and main_gui to fix GUI launch
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,23 +457,62 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.3</v>
+        <v>5.12</v>
       </c>
       <c r="C2" t="n">
-        <v>0.65</v>
+        <v>2.56</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Clustering</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>Random Forest</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>1.42</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.71</v>
+      <c r="B4" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Random Forest</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cross-Validation - Decision Tree</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>